<commit_message>
3 classifiers result were aggregated in the CASS_DB, late fusion was analyzed in case of no test data.
</commit_message>
<xml_diff>
--- a/CASS_DB.xlsx
+++ b/CASS_DB.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bijanmehr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Education\3_ASD classification -Bijan thesis\CASS_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{715C097D-F477-4933-B6F5-2693EFAB6B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1F7767-6A04-4FF1-A3FB-DFAE039C43C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{13C86E0F-BADF-4E14-BE62-16035DC6952A}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13667" activeTab="2" xr2:uid="{13C86E0F-BADF-4E14-BE62-16035DC6952A}"/>
   </bookViews>
   <sheets>
-    <sheet name="LightWheel" sheetId="1" r:id="rId1"/>
-    <sheet name="Parrot" sheetId="2" r:id="rId2"/>
-    <sheet name="Smart car" sheetId="5" r:id="rId3"/>
+    <sheet name="all_classifiers" sheetId="6" r:id="rId1"/>
+    <sheet name="LightWheel" sheetId="1" r:id="rId2"/>
+    <sheet name="Parrot" sheetId="2" r:id="rId3"/>
+    <sheet name="Smart car" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="43">
   <si>
     <t>id</t>
   </si>
@@ -156,6 +157,15 @@
   </si>
   <si>
     <t>result mean pooling</t>
+  </si>
+  <si>
+    <t>result_LW</t>
+  </si>
+  <si>
+    <t>result_P</t>
+  </si>
+  <si>
+    <t>result_SC</t>
   </si>
 </sst>
 </file>
@@ -546,23 +556,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36609C82-F192-4FC6-862C-23580658107B}">
-  <dimension ref="A1:N25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21138527-210D-4C44-9641-4830E4558549}">
+  <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.88671875" customWidth="1"/>
+    <col min="4" max="4" width="20.44140625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -570,160 +578,101 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>94</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>6845</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <f>ROUNDUP(E2*100,2)</f>
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>114</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3">
-        <v>2</v>
-      </c>
-      <c r="D3">
-        <v>6847</v>
-      </c>
-      <c r="E3">
-        <v>2.9209899999999998E-4</v>
-      </c>
-      <c r="F3">
-        <f>ROUNDUP(E3*100,2)</f>
-        <v>0.03</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>120</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>2844</v>
-      </c>
-      <c r="E4">
-        <v>3.5161699999999998E-4</v>
-      </c>
-      <c r="F4">
-        <f>ROUNDUP(E4*100,2)</f>
-        <v>0.04</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>108</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
       <c r="D5">
-        <v>6846</v>
+        <v>1</v>
       </c>
       <c r="E5">
-        <v>5.84283E-4</v>
-      </c>
-      <c r="F5">
-        <f>ROUNDUP(E5*100,2)</f>
-        <v>6.0000000000000005E-2</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>124</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D6">
-        <v>6848</v>
+        <v>1</v>
       </c>
       <c r="E6">
-        <v>2.336449E-3</v>
-      </c>
-      <c r="F6">
-        <f>ROUNDUP(E6*100,2)</f>
-        <v>0.24000000000000002</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>102</v>
       </c>
@@ -731,420 +680,794 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>6847</v>
+        <v>0</v>
       </c>
       <c r="E7">
-        <v>2.6288890000000001E-3</v>
-      </c>
-      <c r="F7">
-        <f>ROUNDUP(E7*100,2)</f>
-        <v>0.27</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>89</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="C8">
-        <v>23</v>
-      </c>
-      <c r="D8">
-        <v>6849</v>
-      </c>
-      <c r="E8">
-        <v>3.3581539999999999E-3</v>
-      </c>
-      <c r="F8">
-        <f>ROUNDUP(E8*100,2)</f>
-        <v>0.34</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>110</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <f ca="1">-E10</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13">
         <v>116</v>
       </c>
-      <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>24</v>
-      </c>
-      <c r="D9">
-        <v>6859</v>
-      </c>
-      <c r="E9">
-        <v>3.4990519999999999E-3</v>
-      </c>
-      <c r="F9">
-        <f>ROUNDUP(E9*100,2)</f>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>112</v>
-      </c>
-      <c r="B10" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10">
-        <v>31</v>
-      </c>
-      <c r="D10">
-        <v>5526</v>
-      </c>
-      <c r="E10">
-        <v>5.6098440000000001E-3</v>
-      </c>
-      <c r="F10">
-        <f>ROUNDUP(E10*100,2)</f>
-        <v>0.57000000000000006</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>95</v>
-      </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>68</v>
-      </c>
-      <c r="D11">
-        <v>6852</v>
-      </c>
-      <c r="E11">
-        <v>9.9241099999999999E-3</v>
-      </c>
-      <c r="F11">
-        <f>ROUNDUP(E11*100,2)</f>
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>87</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>92</v>
-      </c>
-      <c r="D12">
-        <v>5200</v>
-      </c>
-      <c r="E12">
-        <v>1.7692308E-2</v>
-      </c>
-      <c r="F12">
-        <f>ROUNDUP(E12*100,2)</f>
-        <v>1.77</v>
-      </c>
-      <c r="G12">
-        <v>1</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>106</v>
-      </c>
       <c r="B13" t="s">
         <v>5</v>
       </c>
       <c r="C13">
-        <v>132</v>
+        <v>0</v>
       </c>
       <c r="D13">
-        <v>6848</v>
+        <v>1</v>
       </c>
       <c r="E13">
-        <v>1.9275700999999999E-2</v>
-      </c>
-      <c r="F13">
-        <f>ROUNDUP(E13*100,2)</f>
-        <v>1.93</v>
-      </c>
-      <c r="G13">
-        <v>1</v>
-      </c>
-      <c r="H13" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14">
+        <v>118</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>120</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16">
         <v>121</v>
       </c>
-      <c r="B14" t="s">
-        <v>6</v>
-      </c>
-      <c r="C14">
-        <v>154</v>
-      </c>
-      <c r="D14">
-        <v>5350</v>
-      </c>
-      <c r="E14">
-        <v>2.8785047000000001E-2</v>
-      </c>
-      <c r="F14">
-        <f>ROUNDUP(E14*100,2)</f>
-        <v>2.88</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>118</v>
-      </c>
-      <c r="B15" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15">
-        <v>479</v>
-      </c>
-      <c r="D15">
-        <v>6849</v>
-      </c>
-      <c r="E15">
-        <v>6.9937216999999996E-2</v>
-      </c>
-      <c r="F15">
-        <f>ROUNDUP(E15*100,2)</f>
-        <v>7</v>
-      </c>
-      <c r="G15">
-        <v>1</v>
-      </c>
-      <c r="H15">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>110</v>
-      </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>799</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>6847</v>
+        <v>2</v>
       </c>
       <c r="E16">
-        <v>0.11669344199999999</v>
-      </c>
-      <c r="F16">
-        <f>ROUNDUP(E16*100,2)</f>
-        <v>11.67</v>
-      </c>
-      <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>100</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>1381</v>
+        <v>0</v>
       </c>
       <c r="D17">
-        <v>6843</v>
+        <v>0</v>
       </c>
       <c r="E17">
-        <v>0.20181207100000001</v>
-      </c>
-      <c r="F17">
-        <f>ROUNDUP(E17*100,2)</f>
-        <v>20.190000000000001</v>
-      </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H20" t="s">
-        <v>29</v>
-      </c>
-      <c r="I20">
-        <v>3.6259999999999999</v>
-      </c>
-      <c r="J20" s="8">
-        <v>0.54714285714285715</v>
-      </c>
-      <c r="L20" t="s">
-        <v>32</v>
-      </c>
-      <c r="M20">
-        <v>1.77</v>
-      </c>
-      <c r="N20" s="8">
-        <v>0.24</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21">
-        <v>0.54714285714285715</v>
-      </c>
-      <c r="J21" s="8">
-        <v>1.1629142857142858</v>
-      </c>
-      <c r="L21" t="s">
-        <v>33</v>
-      </c>
-      <c r="M21">
-        <v>0.24000000000000002</v>
-      </c>
-      <c r="N21" s="8">
-        <v>0.54600000000000004</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="H22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I22">
-        <v>0.61577142857142864</v>
-      </c>
-      <c r="J22" s="8">
-        <v>1.7786857142857144</v>
-      </c>
-      <c r="L22" t="s">
-        <v>31</v>
-      </c>
-      <c r="M22">
-        <v>0.30599999999999999</v>
-      </c>
-      <c r="N22" s="8">
-        <v>0.85200000000000009</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J23" s="8">
-        <v>2.3944571428571431</v>
-      </c>
-      <c r="N23" s="8">
-        <v>1.1580000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J24" s="8">
-        <v>3.0102285714285717</v>
-      </c>
-      <c r="N24" s="8">
-        <v>1.4640000000000002</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="J25" s="8">
-        <v>3.6259999999999999</v>
-      </c>
-      <c r="N25" s="8">
-        <v>1.7700000000000002</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G17">
-    <sortCondition ref="F5:F17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C17">
+    <sortCondition ref="A5:A17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36609C82-F192-4FC6-862C-23580658107B}">
+  <dimension ref="A1:N25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.33203125" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.109375" customWidth="1"/>
+    <col min="12" max="12" width="15.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>87</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>92</v>
+      </c>
+      <c r="D2">
+        <v>5200</v>
+      </c>
+      <c r="E2">
+        <v>1.7692308E-2</v>
+      </c>
+      <c r="F2">
+        <f>ROUNDUP(E2*100,2)</f>
+        <v>1.77</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>89</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3">
+        <v>23</v>
+      </c>
+      <c r="D3">
+        <v>6849</v>
+      </c>
+      <c r="E3">
+        <v>3.3581539999999999E-3</v>
+      </c>
+      <c r="F3">
+        <f>ROUNDUP(E3*100,2)</f>
+        <v>0.34</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>6845</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <f>ROUNDUP(E4*100,2)</f>
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>68</v>
+      </c>
+      <c r="D5">
+        <v>6852</v>
+      </c>
+      <c r="E5">
+        <v>9.9241099999999999E-3</v>
+      </c>
+      <c r="F5">
+        <f>ROUNDUP(E5*100,2)</f>
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1381</v>
+      </c>
+      <c r="D6">
+        <v>6843</v>
+      </c>
+      <c r="E6">
+        <v>0.20181207100000001</v>
+      </c>
+      <c r="F6">
+        <f>ROUNDUP(E6*100,2)</f>
+        <v>20.190000000000001</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>102</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7">
+        <v>18</v>
+      </c>
+      <c r="D7">
+        <v>6847</v>
+      </c>
+      <c r="E7">
+        <v>2.6288890000000001E-3</v>
+      </c>
+      <c r="F7">
+        <f>ROUNDUP(E7*100,2)</f>
+        <v>0.27</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8">
+        <v>132</v>
+      </c>
+      <c r="D8">
+        <v>6848</v>
+      </c>
+      <c r="E8">
+        <v>1.9275700999999999E-2</v>
+      </c>
+      <c r="F8">
+        <f>ROUNDUP(E8*100,2)</f>
+        <v>1.93</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+      <c r="D9">
+        <v>6846</v>
+      </c>
+      <c r="E9">
+        <v>5.84283E-4</v>
+      </c>
+      <c r="F9">
+        <f>ROUNDUP(E9*100,2)</f>
+        <v>6.0000000000000005E-2</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>110</v>
+      </c>
+      <c r="B10" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10">
+        <v>799</v>
+      </c>
+      <c r="D10">
+        <v>6847</v>
+      </c>
+      <c r="E10">
+        <v>0.11669344199999999</v>
+      </c>
+      <c r="F10">
+        <f>ROUNDUP(E10*100,2)</f>
+        <v>11.67</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>31</v>
+      </c>
+      <c r="D11">
+        <v>5526</v>
+      </c>
+      <c r="E11">
+        <v>5.6098440000000001E-3</v>
+      </c>
+      <c r="F11">
+        <f>ROUNDUP(E11*100,2)</f>
+        <v>0.57000000000000006</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>114</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12">
+        <v>6847</v>
+      </c>
+      <c r="E12">
+        <v>2.9209899999999998E-4</v>
+      </c>
+      <c r="F12">
+        <f>ROUNDUP(E12*100,2)</f>
+        <v>0.03</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>116</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13">
+        <v>24</v>
+      </c>
+      <c r="D13">
+        <v>6859</v>
+      </c>
+      <c r="E13">
+        <v>3.4990519999999999E-3</v>
+      </c>
+      <c r="F13">
+        <f>ROUNDUP(E13*100,2)</f>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>118</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>479</v>
+      </c>
+      <c r="D14">
+        <v>6849</v>
+      </c>
+      <c r="E14">
+        <v>6.9937216999999996E-2</v>
+      </c>
+      <c r="F14">
+        <f>ROUNDUP(E14*100,2)</f>
+        <v>7</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>120</v>
+      </c>
+      <c r="B15" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>2844</v>
+      </c>
+      <c r="E15">
+        <v>3.5161699999999998E-4</v>
+      </c>
+      <c r="F15">
+        <f>ROUNDUP(E15*100,2)</f>
+        <v>0.04</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>121</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>154</v>
+      </c>
+      <c r="D16">
+        <v>5350</v>
+      </c>
+      <c r="E16">
+        <v>2.8785047000000001E-2</v>
+      </c>
+      <c r="F16">
+        <f>ROUNDUP(E16*100,2)</f>
+        <v>2.88</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>124</v>
+      </c>
+      <c r="B17" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>6848</v>
+      </c>
+      <c r="E17">
+        <v>2.336449E-3</v>
+      </c>
+      <c r="F17">
+        <f>ROUNDUP(E17*100,2)</f>
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H20" t="s">
+        <v>29</v>
+      </c>
+      <c r="I20">
+        <v>3.6259999999999999</v>
+      </c>
+      <c r="J20" s="8">
+        <v>0.54714285714285715</v>
+      </c>
+      <c r="L20" t="s">
+        <v>32</v>
+      </c>
+      <c r="M20">
+        <v>1.77</v>
+      </c>
+      <c r="N20" s="8">
+        <v>0.24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H21" t="s">
+        <v>30</v>
+      </c>
+      <c r="I21">
+        <v>0.54714285714285715</v>
+      </c>
+      <c r="J21" s="8">
+        <v>1.1629142857142858</v>
+      </c>
+      <c r="L21" t="s">
+        <v>33</v>
+      </c>
+      <c r="M21">
+        <v>0.24000000000000002</v>
+      </c>
+      <c r="N21" s="8">
+        <v>0.54600000000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I22">
+        <v>0.61577142857142864</v>
+      </c>
+      <c r="J22" s="8">
+        <v>1.7786857142857144</v>
+      </c>
+      <c r="L22" t="s">
+        <v>31</v>
+      </c>
+      <c r="M22">
+        <v>0.30599999999999999</v>
+      </c>
+      <c r="N22" s="8">
+        <v>0.85200000000000009</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J23" s="8">
+        <v>2.3944571428571431</v>
+      </c>
+      <c r="N23" s="8">
+        <v>1.1580000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J24" s="8">
+        <v>3.0102285714285717</v>
+      </c>
+      <c r="N24" s="8">
+        <v>1.4640000000000002</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J25" s="8">
+        <v>3.6259999999999999</v>
+      </c>
+      <c r="N25" s="8">
+        <v>1.7700000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H17">
+    <sortCondition ref="A2:A17"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61C73FCE-D443-42D7-AA21-554D4171C054}">
   <dimension ref="A1:Q36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13:J13"/>
+      <selection activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.88671875" customWidth="1"/>
     <col min="5" max="5" width="18" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.7109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.44140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1197,7 +1520,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>87</v>
       </c>
@@ -1214,7 +1537,7 @@
         <v>0.69631100000000001</v>
       </c>
       <c r="F2" s="2">
-        <f>MAX(C2:E2)</f>
+        <f t="shared" ref="F2:F15" si="0">MAX(C2:E2)</f>
         <v>0.82242499999999996</v>
       </c>
       <c r="G2" s="2">
@@ -1253,7 +1576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>89</v>
       </c>
@@ -1270,7 +1593,7 @@
         <v>0.58191400000000004</v>
       </c>
       <c r="F3" s="2">
-        <f>MAX(C3:E3)</f>
+        <f t="shared" si="0"/>
         <v>0.90913699999999997</v>
       </c>
       <c r="G3" s="2">
@@ -1286,7 +1609,7 @@
         <v>0.38796799999999998</v>
       </c>
       <c r="K3" s="4">
-        <f t="shared" ref="K3:K17" si="0">MAX(H3:J3)</f>
+        <f t="shared" ref="K3:K17" si="1">MAX(H3:J3)</f>
         <v>0.67254800000000003</v>
       </c>
       <c r="L3" s="4">
@@ -1302,14 +1625,14 @@
         <v>0.39385999999999999</v>
       </c>
       <c r="P3" s="6">
-        <f t="shared" ref="P3:P17" si="1">MAX(M3:O3)</f>
+        <f t="shared" ref="P3:P17" si="2">MAX(M3:O3)</f>
         <v>0.57254799999999995</v>
       </c>
       <c r="Q3" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>94</v>
       </c>
@@ -1326,7 +1649,7 @@
         <v>0.58191400000000004</v>
       </c>
       <c r="F4" s="2">
-        <f>MAX(C4:E4)</f>
+        <f t="shared" si="0"/>
         <v>0.90913699999999997</v>
       </c>
       <c r="G4" s="2">
@@ -1342,7 +1665,7 @@
         <v>0.37051400000000001</v>
       </c>
       <c r="K4" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.71611599999999997</v>
       </c>
       <c r="L4" s="4">
@@ -1358,14 +1681,14 @@
         <v>0.388679</v>
       </c>
       <c r="P4" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.74740099999999998</v>
       </c>
       <c r="Q4" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>95</v>
       </c>
@@ -1382,7 +1705,7 @@
         <v>0.79504600000000003</v>
       </c>
       <c r="F5" s="2">
-        <f>MAX(C5:E5)</f>
+        <f t="shared" si="0"/>
         <v>0.95173399999999997</v>
       </c>
       <c r="G5" s="2">
@@ -1398,7 +1721,7 @@
         <v>0.57334099999999999</v>
       </c>
       <c r="K5" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.83992999999999995</v>
       </c>
       <c r="L5" s="4">
@@ -1414,14 +1737,14 @@
         <v>0.52165499999999998</v>
       </c>
       <c r="P5" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.87201499999999998</v>
       </c>
       <c r="Q5" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>100</v>
       </c>
@@ -1438,7 +1761,7 @@
         <v>0.84473699999999996</v>
       </c>
       <c r="F6" s="2">
-        <f>MAX(C6:E6)</f>
+        <f t="shared" si="0"/>
         <v>0.96125099999999997</v>
       </c>
       <c r="G6" s="2">
@@ -1454,7 +1777,7 @@
         <v>0.76289700000000005</v>
       </c>
       <c r="K6" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.79393199999999997</v>
       </c>
       <c r="L6" s="4">
@@ -1470,14 +1793,14 @@
         <v>0.61881699999999995</v>
       </c>
       <c r="P6" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.87596399999999996</v>
       </c>
       <c r="Q6" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>102</v>
       </c>
@@ -1494,7 +1817,7 @@
         <v>0.79115500000000005</v>
       </c>
       <c r="F7" s="2">
-        <f>MAX(C7:E7)</f>
+        <f t="shared" si="0"/>
         <v>0.84515399999999996</v>
       </c>
       <c r="G7" s="2">
@@ -1510,7 +1833,7 @@
         <v>7.0542999999999995E-2</v>
       </c>
       <c r="K7" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.74508600000000003</v>
       </c>
       <c r="L7" s="4">
@@ -1526,14 +1849,14 @@
         <v>0.17353199999999999</v>
       </c>
       <c r="P7" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.95385600000000004</v>
       </c>
       <c r="Q7" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>106</v>
       </c>
@@ -1550,7 +1873,7 @@
         <v>0.817913</v>
       </c>
       <c r="F8" s="2">
-        <f>MAX(C8:E8)</f>
+        <f t="shared" si="0"/>
         <v>0.95837300000000003</v>
       </c>
       <c r="G8" s="2">
@@ -1566,7 +1889,7 @@
         <v>0.90639099999999995</v>
       </c>
       <c r="K8" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.90639099999999995</v>
       </c>
       <c r="L8" s="4">
@@ -1582,14 +1905,14 @@
         <v>0.72596899999999998</v>
       </c>
       <c r="P8" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.91473499999999996</v>
       </c>
       <c r="Q8" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>108</v>
       </c>
@@ -1606,7 +1929,7 @@
         <v>0.87287199999999998</v>
       </c>
       <c r="F9" s="2">
-        <f>MAX(C9:E9)</f>
+        <f t="shared" si="0"/>
         <v>0.87287199999999998</v>
       </c>
       <c r="G9" s="2">
@@ -1622,7 +1945,7 @@
         <v>0.82408599999999999</v>
       </c>
       <c r="K9" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.82408599999999999</v>
       </c>
       <c r="L9" s="4">
@@ -1638,14 +1961,14 @@
         <v>0.62507299999999999</v>
       </c>
       <c r="P9" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.79386900000000005</v>
       </c>
       <c r="Q9" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>110</v>
       </c>
@@ -1662,7 +1985,7 @@
         <v>0.74845499999999998</v>
       </c>
       <c r="F10" s="2">
-        <f>MAX(C10:E10)</f>
+        <f t="shared" si="0"/>
         <v>0.84709000000000001</v>
       </c>
       <c r="G10" s="2">
@@ -1678,7 +2001,7 @@
         <v>9.4458799999999996E-2</v>
       </c>
       <c r="K10" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.75675700000000001</v>
       </c>
       <c r="L10" s="4">
@@ -1694,14 +2017,14 @@
         <v>0.33462799999999998</v>
       </c>
       <c r="P10" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.76952500000000001</v>
       </c>
       <c r="Q10" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>112</v>
       </c>
@@ -1718,7 +2041,7 @@
         <v>0.79115500000000005</v>
       </c>
       <c r="F11" s="2">
-        <f>MAX(C11:E11)</f>
+        <f t="shared" si="0"/>
         <v>0.86256699999999997</v>
       </c>
       <c r="G11" s="2">
@@ -1734,7 +2057,7 @@
         <v>0.26847399999999999</v>
       </c>
       <c r="K11" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.66834300000000002</v>
       </c>
       <c r="L11" s="4">
@@ -1750,14 +2073,14 @@
         <v>0.35966900000000002</v>
       </c>
       <c r="P11" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.75444900000000004</v>
       </c>
       <c r="Q11" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>114</v>
       </c>
@@ -1774,7 +2097,7 @@
         <v>0.68041399999999996</v>
       </c>
       <c r="F12" s="2">
-        <f>MAX(C12:E12)</f>
+        <f t="shared" si="0"/>
         <v>0.85041999999999995</v>
       </c>
       <c r="G12" s="2">
@@ -1790,7 +2113,7 @@
         <v>0.15745799999999999</v>
       </c>
       <c r="K12" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.81030800000000003</v>
       </c>
       <c r="L12" s="4">
@@ -1806,14 +2129,14 @@
         <v>0.330287</v>
       </c>
       <c r="P12" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.80952500000000005</v>
       </c>
       <c r="Q12" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>116</v>
       </c>
@@ -1830,7 +2153,7 @@
         <v>0.64149999999999996</v>
       </c>
       <c r="F13" s="2">
-        <f>MAX(C13:E13)</f>
+        <f t="shared" si="0"/>
         <v>0.84632700000000005</v>
       </c>
       <c r="G13" s="2">
@@ -1846,7 +2169,7 @@
         <v>5.2050899999999997E-2</v>
       </c>
       <c r="K13" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.70200600000000002</v>
       </c>
       <c r="L13" s="4">
@@ -1862,14 +2185,14 @@
         <v>0.17330799999999999</v>
       </c>
       <c r="P13" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.412526</v>
       </c>
       <c r="Q13" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>118</v>
       </c>
@@ -1886,7 +2209,7 @@
         <v>0.83333299999999999</v>
       </c>
       <c r="F14" s="2">
-        <f>MAX(C14:E14)</f>
+        <f t="shared" si="0"/>
         <v>0.92574100000000004</v>
       </c>
       <c r="G14" s="2">
@@ -1902,7 +2225,7 @@
         <v>0.30127500000000002</v>
       </c>
       <c r="K14" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.37771500000000002</v>
       </c>
       <c r="L14" s="4">
@@ -1918,14 +2241,14 @@
         <v>0.79511100000000001</v>
       </c>
       <c r="P14" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.79511100000000001</v>
       </c>
       <c r="Q14" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>120</v>
       </c>
@@ -1942,7 +2265,7 @@
         <v>0.33333299999999999</v>
       </c>
       <c r="F15" s="2">
-        <f>MAX(C15:E15)</f>
+        <f t="shared" si="0"/>
         <v>0.33333299999999999</v>
       </c>
       <c r="G15" s="2">
@@ -1958,7 +2281,7 @@
         <v>0.44494800000000001</v>
       </c>
       <c r="K15" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.44494800000000001</v>
       </c>
       <c r="L15" s="4">
@@ -1974,14 +2297,14 @@
         <v>0.77080700000000002</v>
       </c>
       <c r="P15" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.77080700000000002</v>
       </c>
       <c r="Q15" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>121</v>
       </c>
@@ -2034,7 +2357,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>124</v>
       </c>
@@ -2067,7 +2390,7 @@
         <v>0.382685</v>
       </c>
       <c r="K17" s="4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.74599400000000005</v>
       </c>
       <c r="L17" s="4">
@@ -2083,14 +2406,14 @@
         <v>0.249639</v>
       </c>
       <c r="P17" s="6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.78778800000000004</v>
       </c>
       <c r="Q17" s="6">
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -2122,7 +2445,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>87</v>
       </c>
@@ -2158,7 +2481,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>89</v>
       </c>
@@ -2184,14 +2507,14 @@
         <v>1</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22:I36" si="2">AVERAGE(D22,F22,H22)</f>
+        <f>AVERAGE(D22,F22,H22)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J22">
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>94</v>
       </c>
@@ -2217,14 +2540,14 @@
         <v>1</v>
       </c>
       <c r="I23">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D23,F23,H23)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="J23">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>95</v>
       </c>
@@ -2250,14 +2573,14 @@
         <v>1</v>
       </c>
       <c r="I24">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D24,F24,H24)</f>
         <v>1</v>
       </c>
       <c r="J24">
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>100</v>
       </c>
@@ -2283,14 +2606,14 @@
         <v>1</v>
       </c>
       <c r="I25">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D25,F25,H25)</f>
         <v>1</v>
       </c>
       <c r="J25">
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>102</v>
       </c>
@@ -2316,14 +2639,14 @@
         <v>0</v>
       </c>
       <c r="I26">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D26,F26,H26)</f>
         <v>0</v>
       </c>
       <c r="J26">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>106</v>
       </c>
@@ -2349,14 +2672,14 @@
         <v>1</v>
       </c>
       <c r="I27">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D27,F27,H27)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J27">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>108</v>
       </c>
@@ -2382,14 +2705,14 @@
         <v>1</v>
       </c>
       <c r="I28">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D28,F28,H28)</f>
         <v>0.33333333333333331</v>
       </c>
       <c r="J28">
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>110</v>
       </c>
@@ -2415,14 +2738,14 @@
         <v>1</v>
       </c>
       <c r="I29">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D29,F29,H29)</f>
         <v>1</v>
       </c>
       <c r="J29">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>112</v>
       </c>
@@ -2448,14 +2771,14 @@
         <v>1</v>
       </c>
       <c r="I30">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D30,F30,H30)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J30">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>114</v>
       </c>
@@ -2481,14 +2804,14 @@
         <v>1</v>
       </c>
       <c r="I31">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D31,F31,H31)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J31">
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>116</v>
       </c>
@@ -2514,14 +2837,14 @@
         <v>1</v>
       </c>
       <c r="I32">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D32,F32,H32)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J32">
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>118</v>
       </c>
@@ -2547,14 +2870,14 @@
         <v>0</v>
       </c>
       <c r="I33">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D33,F33,H33)</f>
         <v>0.66666666666666663</v>
       </c>
       <c r="J33">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>120</v>
       </c>
@@ -2580,14 +2903,14 @@
         <v>0</v>
       </c>
       <c r="I34">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D34,F34,H34)</f>
         <v>0</v>
       </c>
       <c r="J34">
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>121</v>
       </c>
@@ -2616,7 +2939,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>124</v>
       </c>
@@ -2642,7 +2965,7 @@
         <v>0</v>
       </c>
       <c r="I36">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D36,F36,H36)</f>
         <v>0</v>
       </c>
       <c r="J36">
@@ -2650,28 +2973,28 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E17">
-    <sortCondition ref="A2:A17"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A21:K36">
+    <sortCondition ref="A21:A36"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{855A4EF6-274C-4322-B3AD-46C986856F78}">
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2685,37 +3008,37 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>121</v>
+        <v>87</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>7.36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>84.39</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>124</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>11.73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>13.72</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
@@ -2724,122 +3047,123 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>13.72</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38.31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5">
+        <v>71.94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6">
+        <v>79.260000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
         <v>102</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
         <v>24.18</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>94</v>
-      </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>38.31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>118</v>
-      </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>41.78</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8">
-        <v>60.83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>97.11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9">
-        <v>71.94</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
       <c r="C10">
-        <v>1</v>
+        <f ca="1">-C10</f>
+        <v>0</v>
       </c>
       <c r="D10">
-        <v>79.260000000000005</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>91.07</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
+        <v>112</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>98.57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
         <v>114</v>
       </c>
-      <c r="B11" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11">
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
         <v>81.55</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>87</v>
-      </c>
-      <c r="B12" t="s">
-        <v>5</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>84.39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>116</v>
       </c>
@@ -2853,66 +3177,65 @@
         <v>86.04</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>110</v>
+        <v>118</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
       <c r="C14">
-        <f ca="1">-C14</f>
         <v>0</v>
       </c>
       <c r="D14">
-        <v>91.07</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41.78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>106</v>
+        <v>120</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15">
-        <v>97.11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>60.83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D16">
-        <v>98.57</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>7.36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="B17" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
-        <v>37</v>
+        <v>8</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>11.73</v>
       </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D17">
-    <sortCondition ref="D2:D17"/>
+    <sortCondition ref="A1:A17"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>